<commit_message>
Update whole filiere structure through XLSX file
</commit_message>
<xml_diff>
--- a/GestionNote/src/main/resources/new_filiere_structure.xlsx
+++ b/GestionNote/src/main/resources/new_filiere_structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xd-11\Documents\GitHub\gestion_notes\gestion_des_notes\GestionNote\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66122E6C-55D0-49AD-A117-16D54D0B5152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99286F7E-D3DB-4FBF-899E-69640F32E5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{21A2383F-5E3C-4579-9F45-4E91C7FB34DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{21A2383F-5E3C-4579-9F45-4E91C7FB34DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Filiere" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,222 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Younes Khoubaz</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{205CCFBC-93CE-4BF1-B967-BBA8131A619B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+valid formats:
+dd-MM-yyyy
+dd/MM/yyyy
+yyyy-MM-dd
+yyyy/MM/dd</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{0C88B5C5-A123-4F2A-87DA-1EF8CBBBD9AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+valid formats:
+dd-MM-yyyy
+dd/MM/yyyy
+yyyy-MM-dd
+yyyy/MM/dd</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{9EE53A54-9C54-4709-83AD-65E1061B3849}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If the professor’s data already exists, the CIN is enough</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Younes Khoubaz</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{57C119C6-388E-46C9-A0FD-E529370076CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+A number representing the level's order (1: first year, 2: second year…)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Younes Khoubaz</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{691CFF76-6884-4C6F-9584-1B909BE8EB15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Level alias in which the module belongs</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{85E95944-36AC-4494-847F-CFFB1E0D4785}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If the professor’s data already exists, the CIN is enough</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Younes Khoubaz</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{5CA43FCB-A0EF-4D9B-8D34-85A7BD9C7AEC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Younes Khoubaz:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Module code in which the element belongs</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
@@ -68,9 +284,6 @@
     <t>Coordinator Phone</t>
   </si>
   <si>
-    <t>YYYY-MM-DD</t>
-  </si>
-  <si>
     <t>Order</t>
   </si>
   <si>
@@ -96,13 +309,16 @@
   </si>
   <si>
     <t>Module Code</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +333,32 @@
       <family val="2"/>
       <charset val="178"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -160,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,6 +414,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -507,11 +752,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3D407D-BC7C-4C32-A033-F33D529638C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3D407D-BC7C-4C32-A033-F33D529638C4}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -559,11 +804,11 @@
     <row r="2" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+      <c r="C2" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -573,15 +818,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA653345-A677-4E10-9EDE-FE84A361D172}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA653345-A677-4E10-9EDE-FE84A361D172}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -599,7 +845,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
@@ -622,15 +868,16 @@
     <row r="6" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA75D42D-535F-4F26-889E-BDDD11F9BE5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA75D42D-535F-4F26-889E-BDDD11F9BE5E}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -649,38 +896,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AE1876-C4F7-4875-B6E0-1A040F5AF6AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AE1876-C4F7-4875-B6E0-1A040F5AF6AA}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -689,16 +937,17 @@
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="25.8" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>